<commit_message>
on adding tp4 set memo on 21.02
</commit_message>
<xml_diff>
--- a/emp list.xlsx
+++ b/emp list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\Desktop\gitdirect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803BC084-EF52-462D-A339-22AA183C32B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5730D7E-7BC0-4FB4-AB94-8F5C154F1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{A6B46598-801A-48E1-B4C7-5D79048F9374}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A6B46598-801A-48E1-B4C7-5D79048F9374}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -923,13 +923,13 @@
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -937,7 +937,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -945,7 +945,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -953,7 +953,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -961,7 +961,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -969,7 +969,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -977,7 +977,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -985,7 +985,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -993,7 +993,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1201,12 +1201,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>25</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -1414,262 +1414,262 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>110</v>
       </c>
@@ -1686,18 +1686,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF4860-9E81-43E6-BCB2-347699814093}">
   <dimension ref="A1:J175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B158" workbookViewId="0">
-      <selection activeCell="J168" sqref="J168"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="4" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>&lt;option value="A Anuradha"&gt;A Anuradha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>&lt;option value="A Mani"&gt;A Mani&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>&lt;option value="A Purusotham Raju"&gt;A Purusotham Raju&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>&lt;option value="AP Subbarayudu"&gt;AP Subbarayudu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>&lt;option value="B Devaraja"&gt;B Devaraja&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>&lt;option value="B Gangadhar"&gt;B Gangadhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>171</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>&lt;option value="B Kalyan Kumar"&gt;B Kalyan Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>&lt;option value="B Lokanath Reddy"&gt;B Lokanath Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>&lt;option value="B Mahesh"&gt;B Mahesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>&lt;option value="B Md Rafi"&gt;B Md Rafi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>&lt;option value="B Nagamma"&gt;B Nagamma&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>&lt;option value="B Raghuram Naik"&gt;B Raghuram Naik&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>&lt;option value="B Raja Naik"&gt;B Raja Naik&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>&lt;option value="B Ramesh Raju"&gt;B Ramesh Raju&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>&lt;option value="B Sai Ganesh"&gt;B Sai Ganesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>&lt;option value="B Sreekanth Babu"&gt;B Sreekanth Babu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>&lt;option value="B Srilatha"&gt;B Srilatha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>&lt;option value="B Srinivasulu"&gt;B Srinivasulu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>&lt;option value="B Venu"&gt;B Venu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>169</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>&lt;option value="B Vishnu Priya"&gt;B Vishnu Priya&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>&lt;option value="BBS Reddy"&gt;BBS Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>126</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>&lt;option value="BV Reddy"&gt;BV Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>&lt;option value="C Doraswamy"&gt;C Doraswamy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>&lt;option value="C Haridas Reddy"&gt;C Haridas Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>&lt;option value="C Nirmala"&gt;C Nirmala&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>&lt;option value="C Rupesh Chandra"&gt;C Rupesh Chandra&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>&lt;option value="CH Lakshmi Devi"&gt;CH Lakshmi Devi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>&lt;option value="CH Sai Kiran"&gt;CH Sai Kiran&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>168</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>&lt;option value="D Aruna"&gt;D Aruna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>&lt;option value="D Durga Prasad"&gt;D Durga Prasad&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>&lt;option value="D Nandana Kumari"&gt;D Nandana Kumari&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>167</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>&lt;option value="D Sanjith Kumar"&gt;D Sanjith Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>&lt;option value="D Srinu Naik"&gt;D Srinu Naik&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>&lt;option value="E Jyoti"&gt;E Jyoti&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>&lt;option value="E Murali"&gt;E Murali&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>101</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>&lt;option value="G Ashok Kumar"&gt;G Ashok Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>120</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>&lt;option value="G Bala Krishna"&gt;G Bala Krishna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>165</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>&lt;option value="G Bala Surendra"&gt;G Bala Surendra&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>&lt;option value="G Ekambaram"&gt;G Ekambaram&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>&lt;option value="G Ganesh"&gt;G Ganesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>119</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>&lt;option value="G Geeva"&gt;G Geeva&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>97</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>&lt;option value="G Giri Prasad"&gt;G Giri Prasad&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>&lt;option value="G Karthik"&gt;G Karthik&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>173</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>&lt;option value="G Kulai Basha"&gt;G Kulai Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>&lt;option value="G Roop Sekhar"&gt;G Roop Sekhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>&lt;option value="G Sai Madhavi"&gt;G Sai Madhavi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>&lt;option value="G Veeresh Babu"&gt;G Veeresh Babu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>&lt;option value="G Vijay Kumar"&gt;G Vijay Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>&lt;option value="I Naveen Reddy"&gt;I Naveen Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>&lt;option value="I Sasi Rekha"&gt;I Sasi Rekha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>&lt;option value="J Dilli Babu"&gt;J Dilli Babu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>&lt;option value="J Murali Babu"&gt;J Murali Babu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>&lt;option value="K Adi Narayana"&gt;K Adi Narayana&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>&lt;option value="K Babu Reddy"&gt;K Babu Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>&lt;option value="K Bhargava Varma"&gt;K Bhargava Varma&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>118</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>&lt;option value="K Chinnaiah"&gt;K Chinnaiah&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>&lt;option value="K Ganga"&gt;K Ganga&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>&lt;option value="K Lokesh"&gt;K Lokesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>&lt;option value="K Nagaraju"&gt;K Nagaraju&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>&lt;option value="K Nagendra"&gt;K Nagendra&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>52</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>&lt;option value="K Pavan Singh"&gt;K Pavan Singh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>&lt;option value="K Poorna"&gt;K Poorna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>163</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>&lt;option value="K Poornima"&gt;K Poornima&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>&lt;option value="K Rajendran"&gt;K Rajendran&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>&lt;option value="K Rakesh"&gt;K Rakesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>&lt;option value="K Ramanjulu"&gt;K Ramanjulu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>162</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>&lt;option value="K Sai Durga"&gt;K Sai Durga&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>&lt;option value="K Saravana"&gt;K Saravana&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>95</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>&lt;option value="K Shiva Kumar"&gt;K Shiva Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>161</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>&lt;option value="K Srikanth"&gt;K Srikanth&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>116</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>&lt;option value="K Srinivasulu"&gt;K Srinivasulu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>160</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>&lt;option value="K Sunil"&gt;K Sunil&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>&lt;option value="K Suresh"&gt;K Suresh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>&lt;option value="L Pranav"&gt;L Pranav&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>&lt;option value="M Bharath Kumar"&gt;M Bharath Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>&lt;option value="M Chandra Mouli"&gt;M Chandra Mouli&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>&lt;option value="M Guravaiah"&gt;M Guravaiah&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>114</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>&lt;option value="M Harish"&gt;M Harish&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>&lt;option value="M Jayaram"&gt;M Jayaram&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>&lt;option value="M Kishore"&gt;M Kishore&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>&lt;option value="M Kupendra Kumar Rao"&gt;M Kupendra Kumar Rao&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>147</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>&lt;option value="M Muni Reddy"&gt;M Muni Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>&lt;option value="M Nagesh"&gt;M Nagesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>&lt;option value="M Nirmala"&gt;M Nirmala&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>&lt;option value="M Rupesh Kumar"&gt;M Rupesh Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>104</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>&lt;option value="M Saraswathi"&gt;M Saraswathi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>27</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>&lt;option value="M Sri Hari"&gt;M Sri Hari&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>74</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>&lt;option value="M Thej Kumar"&gt;M Thej Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>&lt;option value="M Vasanth Kumar"&gt;M Vasanth Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>&lt;option value="M Venkatesh"&gt;M Venkatesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>146</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>&lt;option value="MV Ramana Murthy"&gt;MV Ramana Murthy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>&lt;option value="N Anjaneyulu"&gt;N Anjaneyulu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>158</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>&lt;option value="N Aruna Jyoti"&gt;N Aruna Jyoti&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>23</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>&lt;option value="N Ashok Kumar"&gt;N Ashok Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>&lt;option value="N Hari Krishna"&gt;N Hari Krishna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>&lt;option value="N Hari Prasad"&gt;N Hari Prasad&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>&lt;option value="N Manjula Reddy"&gt;N Manjula Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>145</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>&lt;option value="N Murali Prasad"&gt;N Murali Prasad&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>157</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>&lt;option value="N Neeraja"&gt;N Neeraja&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>91</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>&lt;option value="N Om Shankar"&gt;N Om Shankar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>156</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>&lt;option value="N Pradeep"&gt;N Pradeep&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>&lt;option value="N Raja Sekhar"&gt;N Raja Sekhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>87</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>&lt;option value="N Shiva"&gt;N Shiva&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>&lt;option value="N Sridhar"&gt;N Sridhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>&lt;option value="N Subramanyam"&gt;N Subramanyam&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>71</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>&lt;option value="N Subramanyam Reddy"&gt;N Subramanyam Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>155</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>&lt;option value="N Sudharshan"&gt;N Sudharshan&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>144</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>&lt;option value="N Vani"&gt;N Vani&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>&lt;option value="P Archana"&gt;P Archana&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>151</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>&lt;option value="P Bramaiah Shetty"&gt;P Bramaiah Shetty&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>55</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>&lt;option value="P Chandraiah"&gt;P Chandraiah&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>60</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>&lt;option value="P Dheeren"&gt;P Dheeren&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>143</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>&lt;option value="P Jayamma"&gt;P Jayamma&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>69</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>&lt;option value="P Koteswara Sharma"&gt;P Koteswara Sharma&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>64</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>&lt;option value="P Mahaboob Basha"&gt;P Mahaboob Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>43</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>&lt;option value="P Mahaboob Sharief"&gt;P Mahaboob Sharief&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>153</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>&lt;option value="P Muni Lakshmi"&gt;P Muni Lakshmi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>77</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>&lt;option value="P Parthasarathy"&gt;P Parthasarathy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>174</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>&lt;option value="P Pratap Reddy"&gt;P Pratap Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>75</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>&lt;option value="P Purnima"&gt;P Purnima&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>94</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>&lt;option value="P Ravi"&gt;P Ravi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>72</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>&lt;option value="P Subbaiah"&gt;P Subbaiah&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>&lt;option value="P Sudharshan"&gt;P Sudharshan&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>&lt;option value="P Sunil Kumar Reddy"&gt;P Sunil Kumar Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>&lt;option value="P Uma Maheswar"&gt;P Uma Maheswar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>&lt;option value="P Varalakshmi"&gt;P Varalakshmi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>140</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>&lt;option value="P Venkataswamy"&gt;P Venkataswamy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>152</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>&lt;option value="P Venkatesh"&gt;P Venkatesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>25</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>&lt;option value="PY Pavan Kumar Reddy"&gt;PY Pavan Kumar Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>100</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>&lt;option value="R Pedda Reddemma"&gt;R Pedda Reddemma&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>139</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>&lt;option value="R Rajendran"&gt;R Rajendran&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>33</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>&lt;option value="R Sandeep Kumar"&gt;R Sandeep Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>46</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>&lt;option value="R Suresh"&gt;R Suresh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>92</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>&lt;option value="RS Chandra Sekhar"&gt;RS Chandra Sekhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>4</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>&lt;option value="S Chakrapani"&gt;S Chakrapani&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>&lt;option value="S Geetha Sri"&gt;S Geetha Sri&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>150</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>&lt;option value="S Lohitha Sri"&gt;S Lohitha Sri&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>26</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>&lt;option value="S Madhan Mohan Reddy"&gt;S Madhan Mohan Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>96</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>&lt;option value="S Mahaboob Basha"&gt;S Mahaboob Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>&lt;option value="S Maruthi Prasad Reddy"&gt;S Maruthi Prasad Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>99</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>&lt;option value="S Mounika"&gt;S Mounika&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>79</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>&lt;option value="S Pravallika Jeevan"&gt;S Pravallika Jeevan&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>138</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>&lt;option value="S Subramanyam"&gt;S Subramanyam&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>&lt;option value="S Suresh Kumar"&gt;S Suresh Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>137</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>&lt;option value="S Usman"&gt;S Usman&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>&lt;option value="S Vamsi Priya"&gt;S Vamsi Priya&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>136</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>&lt;option value="SA Kadher Basha"&gt;SA Kadher Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>134</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>&lt;option value="SKM Basha"&gt;SKM Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>133</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>&lt;option value="SKMD Basha"&gt;SKMD Basha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>86</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>&lt;option value="SSK Gani Reddy"&gt;SSK Gani Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>135</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>&lt;option value="SVT Reddy"&gt;SVT Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>132</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>&lt;option value="T Dilip Kumar"&gt;T Dilip Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>70</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>&lt;option value="T Kannaiah"&gt;T Kannaiah&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>78</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>&lt;option value="T Kavitha"&gt;T Kavitha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>131</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>&lt;option value="T Manoj"&gt;T Manoj&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>36</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>&lt;option value="T Sasi Kumar"&gt;T Sasi Kumar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>65</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>&lt;option value="T Tirumaleswari"&gt;T Tirumaleswari&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>102</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>&lt;option value="U Padmavathi"&gt;U Padmavathi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>130</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>&lt;option value="V Dilli Sekhar"&gt;V Dilli Sekhar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>&lt;option value="V Hari Krishna"&gt;V Hari Krishna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>&lt;option value="V Hari Krishna"&gt;V Hari Krishna&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>89</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>&lt;option value="V Munnelu"&gt;V Munnelu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>50</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>&lt;option value="V Nagendra Babu"&gt;V Nagendra Babu&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>54</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>&lt;option value="V Rajesh"&gt;V Rajesh&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>149</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>&lt;option value="V Ravindra"&gt;V Ravindra&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>31</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>&lt;option value="V Samba Siva Rao"&gt;V Samba Siva Rao&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>148</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>&lt;option value="V Selvi"&gt;V Selvi&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>129</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>&lt;option value="V Subramanyam"&gt;V Subramanyam&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>98</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>&lt;option value="V Suneetha"&gt;V Suneetha&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>&lt;option value="V Trilokeswar"&gt;V Trilokeswar&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>13</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>&lt;option value="VR Siva Narayana"&gt;VR Siva Narayana&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>47</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>&lt;option value="Y Maneendra Reddy"&gt;Y Maneendra Reddy&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>57</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>&lt;option value="Y Purohit"&gt;Y Purohit&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>80</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>&lt;option value="Y Sathish"&gt;Y Sathish&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
on adding mts-2 for tp-4
</commit_message>
<xml_diff>
--- a/emp list.xlsx
+++ b/emp list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms\Desktop\gitdirect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5730D7E-7BC0-4FB4-AB94-8F5C154F1D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90744ACF-9DF4-4473-A5D1-EA795A4B66E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A6B46598-801A-48E1-B4C7-5D79048F9374}"/>
   </bookViews>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF4860-9E81-43E6-BCB2-347699814093}">
   <dimension ref="A1:J175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>